<commit_message>
Set up input data for tests and added applied demand test.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{382E1A28-B847-472B-ADF8-439CE9DEB99A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31778CEC-5A21-4220-8FD6-846DE787B9E4}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView minimized="1" xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="Storage Take Test" sheetId="1" r:id="rId1"/>
@@ -797,7 +797,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,8 @@
         <v>30</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <f>1000000-5</f>
+        <v>999995</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +841,7 @@
       </c>
       <c r="B6">
         <f>B2*B3</f>
-        <v>10</v>
+        <v>99999.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up tests for model logic to confirm remaining demands are accurate after each supply source is delivered.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31778CEC-5A21-4220-8FD6-846DE787B9E4}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EA77FF7-60EE-4BC2-93AA-CBCBE9077E60}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="7980" yWindow="1365" windowWidth="21600" windowHeight="11385" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
-    <sheet name="Storage Take Test" sheetId="1" r:id="rId1"/>
-    <sheet name="Contingency Conservation Test" sheetId="2" r:id="rId2"/>
+    <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
+    <sheet name="test_modelLogic.py" sheetId="2" r:id="rId2"/>
+    <sheet name="TestInputData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -127,9 +128,6 @@
     <t>Test #4</t>
   </si>
   <si>
-    <t>self.modelLogic.appliedDemand_Contractor</t>
-  </si>
-  <si>
     <t>self.modelLogic.contingentConservationUseReduction_Contractor</t>
   </si>
   <si>
@@ -137,6 +135,54 @@
   </si>
   <si>
     <t>self.contingentConservationUseReductionVolume_Contractor</t>
+  </si>
+  <si>
+    <t>demandsToBeMetBySWPCVP</t>
+  </si>
+  <si>
+    <t>appliedDemand</t>
+  </si>
+  <si>
+    <t>Normal or Better Demands (acre-feet/year)</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Hydrologic Year Type at i</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>SWP/CVP Supply</t>
+  </si>
+  <si>
+    <t>Base Local Supply (Total, acre-feet/year)</t>
+  </si>
+  <si>
+    <t>Base Long-term Conservation (acre-feet/year)</t>
+  </si>
+  <si>
+    <t>demandsToBeMetByStorage</t>
+  </si>
+  <si>
+    <t>Value Used In Test</t>
+  </si>
+  <si>
+    <t>demandsToBeMetByContingentOptions</t>
+  </si>
+  <si>
+    <t>Surface initial storage (acre-feet)</t>
+  </si>
+  <si>
+    <t>Groundwater initial storage (acre-feet)</t>
+  </si>
+  <si>
+    <t>Surface max take capacity (acre-feet)</t>
+  </si>
+  <si>
+    <t>Groundwater max take capacity (acre-feet)</t>
   </si>
 </sst>
 </file>
@@ -515,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E00A02-92B2-45FA-989E-1582EB4636F5}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,38 +855,68 @@
       <c r="A1" t="s">
         <v>24</v>
       </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B2">
-        <f>1000000-5</f>
+        <f>TestInputData!B3-TestInputData!B4</f>
         <v>999995</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <f>B2-TestInputData!B5</f>
+        <v>964995</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <f>B3-TestInputData!B6</f>
+        <v>959995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <f>MAX(0, B4-MIN(TestInputData!B8,TestInputData!B10) - MIN(TestInputData!B9,TestInputData!B11))</f>
+        <v>348495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <f>B2*B3</f>
+      <c r="B15">
+        <f>B2*B12</f>
         <v>99999.5</v>
       </c>
     </row>
@@ -848,4 +924,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <f>7*5000</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>516500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>815000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>194300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests for contingency WMOs
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EA77FF7-60EE-4BC2-93AA-CBCBE9077E60}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93988D3C-D2C4-44FB-AA75-6ADD34BE992C}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="1365" windowWidth="21600" windowHeight="11385" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -128,15 +128,6 @@
     <t>Test #4</t>
   </si>
   <si>
-    <t>self.modelLogic.contingentConservationUseReduction_Contractor</t>
-  </si>
-  <si>
-    <t>self.modelLogic.demandsToBeMetByContingentOptions_Contractor</t>
-  </si>
-  <si>
-    <t>self.contingentConservationUseReductionVolume_Contractor</t>
-  </si>
-  <si>
     <t>demandsToBeMetBySWPCVP</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>i</t>
   </si>
   <si>
-    <t>Hydrologic Year Type at i</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -183,6 +171,66 @@
   </si>
   <si>
     <t>Groundwater max take capacity (acre-feet)</t>
+  </si>
+  <si>
+    <t>Use Reduction with Contingency Conservation Campaign (% of Total Applied Use)</t>
+  </si>
+  <si>
+    <t>Contingency Conservation Publicity Campaign Cost ($/capita)</t>
+  </si>
+  <si>
+    <t>Urban Population (thousands)</t>
+  </si>
+  <si>
+    <t>Storage Volume Trigger for Contingency Conservation (AF)</t>
+  </si>
+  <si>
+    <t>Value in test input data</t>
+  </si>
+  <si>
+    <t>Hydrologic Year Type at i = 0</t>
+  </si>
+  <si>
+    <t>contingentWMOsInput_conservation.csv</t>
+  </si>
+  <si>
+    <t>demandsToBeMetByWaterMarketTransfers</t>
+  </si>
+  <si>
+    <t>Shortage Threshold before Water Market Transfer Supplies are Delivered (% of Total Applied Use)</t>
+  </si>
+  <si>
+    <t>Water Market Transfer Loss Factor (%)</t>
+  </si>
+  <si>
+    <t>Transfer Limit for Normal or Better Years (AFY)</t>
+  </si>
+  <si>
+    <t>Transfer Limit for Dry Years (AFY)</t>
+  </si>
+  <si>
+    <t>Transfer Limit for 2 or More Consecutive Years (% of Dry-Year limit defined above)</t>
+  </si>
+  <si>
+    <t>Wet Year Water Market Transfers and Exchanges Supply Unit Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Above Normal Year Water Market Transfers and Exchanges Supply Unit Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Below Normal Year Water Market Transfers and Exchanges Supply Unit Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Dry Year Water Market Transfers and Exchanges Supply Unit Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Critically Dry Year Water Market Transfers and Exchanges Supply Unit Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>contingentWMOsInput_WaterMarketTransfers.csv</t>
+  </si>
+  <si>
+    <t>totalShortage_Contractor</t>
   </si>
 </sst>
 </file>
@@ -193,7 +241,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +260,14 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -244,6 +300,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -561,7 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E00A02-92B2-45FA-989E-1582EB4636F5}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -840,15 +898,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -856,68 +915,61 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <f>TestInputData!B3-TestInputData!B4</f>
+        <v>31</v>
+      </c>
+      <c r="B2" s="7">
+        <f>TestInputData!B4-TestInputData!B5</f>
         <v>999995</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <f>B2-TestInputData!B5</f>
+        <v>30</v>
+      </c>
+      <c r="B3" s="7">
+        <f>B2-TestInputData!B6</f>
         <v>964995</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <f>B3-TestInputData!B6</f>
+        <v>38</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B3-TestInputData!B7</f>
         <v>959995</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <f>MAX(0, B4-MIN(TestInputData!B8,TestInputData!B10) - MIN(TestInputData!B9,TestInputData!B11))</f>
+        <v>40</v>
+      </c>
+      <c r="B5" s="7">
+        <f>MAX(0, B4-MIN(TestInputData!B9,TestInputData!B11) - MIN(TestInputData!B10,TestInputData!B12))</f>
         <v>348495</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <f>B2*B12</f>
-        <v>99999.5</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7">
+        <f>B5-(TestInputData!B15/100 *test_modelLogic.py!B2)</f>
+        <v>298495.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B6 - MIN(B6, TestInputData!B23)</f>
+        <v>297495.25</v>
       </c>
     </row>
   </sheetData>
@@ -928,99 +980,230 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>1000000</v>
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
         <f>7*5000</f>
         <v>35000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
         <v>5000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>516500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9">
-        <v>95000</v>
+        <v>516500</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <v>815000</v>
+        <v>95000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>815000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>194300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>87602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B11">
-        <v>194300</v>
+      <c r="B18">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>468.09353240000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <v>223.87081979999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28">
+        <v>715.70822710000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29">
+        <v>319.9769799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30">
+        <v>1193.9777059999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated elasticity of demands to be unique for each use type
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93988D3C-D2C4-44FB-AA75-6ADD34BE992C}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F954C3A-EDEE-423E-9B51-7B125F8D77CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="2835" yWindow="2370" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -231,6 +231,48 @@
   </si>
   <si>
     <t>totalShortage_Contractor</t>
+  </si>
+  <si>
+    <t>Storage Volume Trigger for Rationing Programs (AF)</t>
+  </si>
+  <si>
+    <t>Cost for Rationing Program ($/capita)</t>
+  </si>
+  <si>
+    <t>Consecutive Year Loss Adjustment (%)</t>
+  </si>
+  <si>
+    <t>Demand Hardening Factor (%)</t>
+  </si>
+  <si>
+    <t>Retail Price ($/AF)</t>
+  </si>
+  <si>
+    <t>contingentWMOsInput_rationingProgram.csv</t>
+  </si>
+  <si>
+    <t>contingentWMOsInput_elasticityofDemand.csv</t>
+  </si>
+  <si>
+    <t>Elasticity of Demand Single Family Residential</t>
+  </si>
+  <si>
+    <t>Elasticity of Demand Industrial</t>
+  </si>
+  <si>
+    <t>Elasticity of Demand Commercial and Governmental</t>
+  </si>
+  <si>
+    <t>Elasticity of Demand Landscape</t>
+  </si>
+  <si>
+    <t>Lower Loss Boundary</t>
+  </si>
+  <si>
+    <t>Upper Loss Boundary</t>
+  </si>
+  <si>
+    <t>Elasticity of Demand Multi-Family Residential</t>
   </si>
 </sst>
 </file>
@@ -291,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -302,6 +344,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -900,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,22 +1023,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1200,6 +1244,112 @@
       </c>
       <c r="B30">
         <v>1193.9777059999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculated total annual cost in contractor loop
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F954C3A-EDEE-423E-9B51-7B125F8D77CB}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E14AA300-B9E5-4B68-BABF-3B46B8BF2464}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2370" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId2"/>
     <sheet name="TestInputData" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1025,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -1356,4 +1357,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8294450-BD26-460E-A24D-95E81C068E8E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started example of PySwarms
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -1,23 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E14AA300-B9E5-4B68-BABF-3B46B8BF2464}"/>
+  <xr:revisionPtr revIDLastSave="924" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE8DD8C-4248-46CD-AFF2-7AD286DF28D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="4605" yWindow="3240" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId2"/>
     <sheet name="TestInputData" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Optimizer" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Optimizer!$B$3:$D$3</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Optimizer!$B$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Optimizer!$C$3</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Optimizer!$D$3</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Optimizer!$E$3</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Optimizer!$F$4</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Optimizer!$F$4</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Optimizer!$B$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Optimizer!$C$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Optimizer!$D$7</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -274,6 +318,33 @@
   </si>
   <si>
     <t>Elasticity of Demand Multi-Family Residential</t>
+  </si>
+  <si>
+    <t>WMO1</t>
+  </si>
+  <si>
+    <t>WMO2</t>
+  </si>
+  <si>
+    <t>WMO3</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Shortage level:</t>
+  </si>
+  <si>
+    <t>Upper Bounds</t>
+  </si>
+  <si>
+    <t>Rationing</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
@@ -284,7 +355,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +379,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1361,15 +1438,104 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8294450-BD26-460E-A24D-95E81C068E8E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <f>B1-SUM(B3:D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <f>B3*20</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>C3*15</f>
+        <v>750</v>
+      </c>
+      <c r="D4">
+        <f>D3*10</f>
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <f>E3*20</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B4:E4)</f>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started connecting PyMoo logic to model logic.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,60 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="924" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE8DD8C-4248-46CD-AFF2-7AD286DF28D5}"/>
+  <xr:revisionPtr revIDLastSave="995" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B849D541-E975-4CB2-8E98-AE3DC7529378}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="3240" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId2"/>
     <sheet name="TestInputData" sheetId="3" r:id="rId3"/>
-    <sheet name="Optimizer" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">Optimizer!$B$3:$D$3</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Optimizer!$B$4</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Optimizer!$C$3</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Optimizer!$D$3</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Optimizer!$E$3</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Optimizer!$F$4</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
-    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Optimizer!$F$4</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Optimizer!$B$7</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Optimizer!$C$7</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Optimizer!$D$7</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -318,33 +273,6 @@
   </si>
   <si>
     <t>Elasticity of Demand Multi-Family Residential</t>
-  </si>
-  <si>
-    <t>WMO1</t>
-  </si>
-  <si>
-    <t>WMO2</t>
-  </si>
-  <si>
-    <t>WMO3</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Shortage level:</t>
-  </si>
-  <si>
-    <t>Upper Bounds</t>
-  </si>
-  <si>
-    <t>Rationing</t>
-  </si>
-  <si>
-    <t>Total Cost</t>
   </si>
 </sst>
 </file>
@@ -355,7 +283,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,12 +307,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -439,6 +361,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1103,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -1434,108 +1360,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8294450-BD26-460E-A24D-95E81C068E8E}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <f>B1-SUM(B3:D3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4">
-        <f>B3*20</f>
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f>C3*15</f>
-        <v>750</v>
-      </c>
-      <c r="D4">
-        <f>D3*10</f>
-        <v>500</v>
-      </c>
-      <c r="E4">
-        <f>E3*20</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <f>SUM(B4:E4)</f>
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more tests through the reliability management costs calculation step.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="995" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B849D541-E975-4CB2-8E98-AE3DC7529378}"/>
+  <xr:revisionPtr revIDLastSave="1273" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E03F6CD-F988-4BC7-BBF1-1A5AC028CB91}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_storageOperations.py" sheetId="1" r:id="rId1"/>
-    <sheet name="test_modelLogic.py" sheetId="2" r:id="rId2"/>
-    <sheet name="TestInputData" sheetId="3" r:id="rId3"/>
+    <sheet name="test_modelLogic.py" sheetId="2" r:id="rId1"/>
+    <sheet name="TestInputData" sheetId="3" r:id="rId2"/>
+    <sheet name="test_storageOperations.py" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -155,9 +155,6 @@
     <t>demandsToBeMetByStorage</t>
   </si>
   <si>
-    <t>Value Used In Test</t>
-  </si>
-  <si>
     <t>demandsToBeMetByContingentOptions</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Storage Volume Trigger for Contingency Conservation (AF)</t>
   </si>
   <si>
-    <t>Value in test input data</t>
-  </si>
-  <si>
     <t>Hydrologic Year Type at i = 0</t>
   </si>
   <si>
@@ -273,17 +267,196 @@
   </si>
   <si>
     <t>Elasticity of Demand Multi-Family Residential</t>
+  </si>
+  <si>
+    <t>Result for test_modelLogic.py</t>
+  </si>
+  <si>
+    <t>swpCVPDeliveryCost_Contractor</t>
+  </si>
+  <si>
+    <t>Water balance input data</t>
+  </si>
+  <si>
+    <t>Groundwater bank put cost</t>
+  </si>
+  <si>
+    <t>Groundwater bank take cost</t>
+  </si>
+  <si>
+    <t>Groundwater Pumping Cost (Base Supply, Single Dry or Better Year Types)</t>
+  </si>
+  <si>
+    <t>Groundwater Pumping Cost (Base Supply, Multi-Dry Year Types)</t>
+  </si>
+  <si>
+    <t>SWP and/or CVP Delivery Cost</t>
+  </si>
+  <si>
+    <t>Cost of M&amp;I potable water treatment</t>
+  </si>
+  <si>
+    <t>Cost of M&amp;I Distribution</t>
+  </si>
+  <si>
+    <t>Wastewater Treatment Cost</t>
+  </si>
+  <si>
+    <t>Fraction of wastewater centrally treated (%)</t>
+  </si>
+  <si>
+    <t>systemOperationsInput_DeliveryCosts.csv</t>
+  </si>
+  <si>
+    <t>waterTreatmentCost_Contractor</t>
+  </si>
+  <si>
+    <t>distributionCost_Contractor</t>
+  </si>
+  <si>
+    <t>wastewaterTreatmentCost_Contractor</t>
+  </si>
+  <si>
+    <t>waterMarketTransferCost_Contractor</t>
+  </si>
+  <si>
+    <t>contingencyWMOs.waterMarketTransferDeliveries_Contractor</t>
+  </si>
+  <si>
+    <t>putGroundwater_Contractor</t>
+  </si>
+  <si>
+    <t>takeGroundwater_Contractor</t>
+  </si>
+  <si>
+    <t>putSurface_Contractor</t>
+  </si>
+  <si>
+    <t>takeSurface_Contractor</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>this function needs a separate test</t>
+  </si>
+  <si>
+    <t>putGroundwaterBankCost</t>
+  </si>
+  <si>
+    <t>takeGroundwaterBankCost</t>
+  </si>
+  <si>
+    <t>Long-term WMO options (input in test_modelLogic.py)</t>
+  </si>
+  <si>
+    <t># Test implementation of planned conservation</t>
+  </si>
+  <si>
+    <t># Test delivery of local supplies</t>
+  </si>
+  <si>
+    <t># Test deliveries of SWP/CVP supplies</t>
+  </si>
+  <si>
+    <t># Test deliveries from storage (groundwater bank and carryover)</t>
+  </si>
+  <si>
+    <t>#Test implementation of Contingent Conservation Programs</t>
+  </si>
+  <si>
+    <t>contingentConservationCost</t>
+  </si>
+  <si>
+    <t># Test delivery of Water Market Transfers</t>
+  </si>
+  <si>
+    <t># Test other delivery reliability costs</t>
+  </si>
+  <si>
+    <t>totalSuppliesDelivered_Contractor</t>
+  </si>
+  <si>
+    <t>totalLocalSupply</t>
+  </si>
+  <si>
+    <t>totalLongtermWMOSupplyIncrementalVolume_Contractor</t>
+  </si>
+  <si>
+    <t>surfaceLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>groundwaterLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>desalinationLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>recycledLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>potableReuseLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>transfersAndExchangesLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>otherSupplyLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>conservationLongTermWMOCost_Contractor</t>
+  </si>
+  <si>
+    <t>Surface Water Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Groundwater Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Desalination Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Recycled Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Potable Reuse Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Transfers and Exchanges Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Other Supply Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>Additional Conservation Cost ($/AF)</t>
+  </si>
+  <si>
+    <t>longtermWMOsInput_supplyCosts.csv</t>
+  </si>
+  <si>
+    <t># Test total reliability cost</t>
+  </si>
+  <si>
+    <t>reliabilityManagementCost_Contractor</t>
+  </si>
+  <si>
+    <t># Test remaining shortages and associated costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="7">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="183" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="184" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="185" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="188" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,13 +484,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -329,11 +514,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -345,9 +531,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,10 +560,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,6 +858,869 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3">
+        <f>TestInputData!B4-TestInputData!B5</f>
+        <v>999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5">
+        <f>TestInputData!B6</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6">
+        <f>8*10</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3">
+        <f>B3-TestInputData!B6-TestInputData!B7</f>
+        <v>964915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="16">
+        <f>10*TestInputData!B61</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="16">
+        <f>10*TestInputData!B62</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="16">
+        <f>10*TestInputData!B63</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="16">
+        <f>10*TestInputData!B64</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="16">
+        <f>10*TestInputData!B65</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="16">
+        <f>10*TestInputData!B66</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="16">
+        <f>10*TestInputData!B67</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="16">
+        <f>10*TestInputData!B68</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B7-TestInputData!B8</f>
+        <v>959915</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="16">
+        <f>(B7-B17)*TestInputData!B15</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="2">
+        <f>MIN(B17,TestInputData!B21,TestInputData!B23)</f>
+        <v>516500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="2">
+        <f>MIN(B17-B21, TestInputData!B22,TestInputData!B24)</f>
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="13">
+        <f>B23*TestInputData!B12</f>
+        <v>19506431.092</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3">
+        <f>B17-B21-B23</f>
+        <v>348415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="7">
+        <f>B26-(TestInputData!B27/100 *test_modelLogic.py!B3)</f>
+        <v>298415.25</v>
+      </c>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="16">
+        <f>TestInputData!B28*TestInputData!B29*1000</f>
+        <v>21900500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="2">
+        <f>MIN(B28, TestInputData!B35)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="14">
+        <f>B31*TestInputData!B38</f>
+        <v>468093.53240000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="2">
+        <f>B5+(B7-B17)+B23+B21+B31+B6</f>
+        <v>652580</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="15">
+        <f>B34*TestInputData!B16</f>
+        <v>249294165.24617001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="15">
+        <f>B34*TestInputData!B17</f>
+        <v>189153045.02617002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="15">
+        <f>B34*(TestInputData!B19/100)*TestInputData!B18</f>
+        <v>79756562.338470995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="15">
+        <f>SUM(B35:B37,B32,B29,B25,B24,B18,B8:B15)</f>
+        <v>560579597.23521113</v>
+      </c>
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="5">
+        <f>B28 - B31</f>
+        <v>297415.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <f>7*5000</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="10">
+        <v>67.76025473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="10">
+        <v>205.33085360000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="10">
+        <v>22.927610130000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="10">
+        <v>382.01318650000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="10">
+        <v>289.85418650000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="10">
+        <v>244.43458989999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>516500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23">
+        <v>815000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>194300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>87602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38">
+        <v>468.09353240000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>223.87081979999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40">
+        <v>715.70822710000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41">
+        <v>319.9769799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>1193.9777059999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E00A02-92B2-45FA-989E-1582EB4636F5}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -941,423 +1999,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7">
-        <f>TestInputData!B4-TestInputData!B5</f>
-        <v>999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="7">
-        <f>B2-TestInputData!B6</f>
-        <v>964995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7">
-        <f>B3-TestInputData!B7</f>
-        <v>959995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="7">
-        <f>MAX(0, B4-MIN(TestInputData!B9,TestInputData!B11) - MIN(TestInputData!B10,TestInputData!B12))</f>
-        <v>348495</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="7">
-        <f>B5-(TestInputData!B15/100 *test_modelLogic.py!B2)</f>
-        <v>298495.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="5">
-        <f>B6 - MIN(B6, TestInputData!B23)</f>
-        <v>297495.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
-  <dimension ref="A1:B46"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6">
-        <f>7*5000</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9">
-        <v>516500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10">
-        <v>95000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11">
-        <v>815000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>194300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17">
-        <v>87602</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26">
-        <v>468.09353240000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27">
-        <v>223.87081979999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28">
-        <v>715.70822710000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29">
-        <v>319.9769799</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30">
-        <v>1193.9777059999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41">
-        <v>-0.12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43">
-        <v>-0.11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added unit tests for economic loss function up to loss for SF. Still need to resolve total economic loss.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jacobsengineering-my.sharepoint.com/personal/kensey_daly_jacobs_com/Documents/Projects/CA_DWR/Water Supply Economic Model/Repository/California-Urban-Water-Management-Economic-Tool/CaUWMET/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repo\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1273" documentId="8_{E973DA5C-48AF-4039-8BCF-ACEA1D406E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E03F6CD-F988-4BC7-BBF1-1A5AC028CB91}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01A5C7D-0098-4DFF-8DC4-8C589B3734F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="2070" yWindow="9675" windowWidth="21600" windowHeight="6120" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -441,20 +441,48 @@
   </si>
   <si>
     <t># Test remaining shortages and associated costs</t>
+  </si>
+  <si>
+    <t>Surface Water Supply (AF)</t>
+  </si>
+  <si>
+    <t>Groundwater Supply  (AF)</t>
+  </si>
+  <si>
+    <t>Desalination Supply (AF)</t>
+  </si>
+  <si>
+    <t>Recycled Supply (AF)</t>
+  </si>
+  <si>
+    <t>Potable Reuse Supply (AF)</t>
+  </si>
+  <si>
+    <t>Transfers and Exchanges Supply (AF)</t>
+  </si>
+  <si>
+    <t>Other Supply (AF)</t>
+  </si>
+  <si>
+    <t>Additional Conservation (AF)</t>
+  </si>
+  <si>
+    <t>Long-term WMO supply volume inputs (input in test file)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="183" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="184" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="185" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="188" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -519,7 +547,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -539,10 +567,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -861,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +924,8 @@
         <v>31</v>
       </c>
       <c r="B3" s="3">
-        <f>TestInputData!B4-TestInputData!B5</f>
-        <v>999995</v>
+        <f>TestInputData!B4-TestInputData!B5 - TestInputData!B78</f>
+        <v>999985</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,7 +958,7 @@
       </c>
       <c r="B7" s="3">
         <f>B3-TestInputData!B6-TestInputData!B7</f>
-        <v>964915</v>
+        <v>964905</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,7 +1045,7 @@
       </c>
       <c r="B17" s="3">
         <f>B7-TestInputData!B8</f>
-        <v>959915</v>
+        <v>959905</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,7 +1125,7 @@
       </c>
       <c r="B26" s="3">
         <f>B17-B21-B23</f>
-        <v>348415</v>
+        <v>348405</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1111,7 +1140,7 @@
       </c>
       <c r="B28" s="7">
         <f>B26-(TestInputData!B27/100 *test_modelLogic.py!B3)</f>
-        <v>298415.25</v>
+        <v>298405.75</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -1184,7 +1213,7 @@
       <c r="A37" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="17">
         <f>B34*(TestInputData!B19/100)*TestInputData!B18</f>
         <v>79756562.338470995</v>
       </c>
@@ -1215,7 +1244,7 @@
       </c>
       <c r="B41" s="5">
         <f>B28 - B31</f>
-        <v>297415.25</v>
+        <v>297405.75</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,6 +1740,75 @@
         <v>130</v>
       </c>
       <c r="B68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added cost of rationing program to reliability management cost function.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repo\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01A5C7D-0098-4DFF-8DC4-8C589B3734F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A6943-D758-4DD8-8C8E-C2E4CEA807AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="9675" windowWidth="21600" windowHeight="6120" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>Long-term WMO supply volume inputs (input in test file)</t>
+  </si>
+  <si>
+    <t>rationingProgramCost_Contractor</t>
   </si>
 </sst>
 </file>
@@ -888,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,36 +1222,45 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="16">
+        <f>TestInputData!B46*TestInputData!B29*1000</f>
+        <v>175204000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>133</v>
       </c>
-      <c r="B39" s="15">
-        <f>SUM(B35:B37,B32,B29,B25,B24,B18,B8:B15)</f>
-        <v>560579597.23521113</v>
-      </c>
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="B40" s="15">
+        <f>SUM(B35:B38,B32,B29,B25,B24,B18,B8:B15)</f>
+        <v>735783597.23521101</v>
+      </c>
+      <c r="C40" s="15"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B42" s="5">
         <f>B28 - B31</f>
         <v>297405.75</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1260,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed unit tests after fixing double counting of long-term conservation.
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repo\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repos\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A6943-D758-4DD8-8C8E-C2E4CEA807AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A88EFB-EDD0-4F1C-926D-B742E9593521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId1"/>
     <sheet name="TestInputData" sheetId="3" r:id="rId2"/>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -338,18 +338,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>this function needs a separate test</t>
-  </si>
-  <si>
     <t>putGroundwaterBankCost</t>
   </si>
   <si>
     <t>takeGroundwaterBankCost</t>
   </si>
   <si>
-    <t>Long-term WMO options (input in test_modelLogic.py)</t>
-  </si>
-  <si>
     <t># Test implementation of planned conservation</t>
   </si>
   <si>
@@ -471,6 +465,9 @@
   </si>
   <si>
     <t>rationingProgramCost_Contractor</t>
+  </si>
+  <si>
+    <t>volumeGroundwaterBank</t>
   </si>
 </sst>
 </file>
@@ -522,18 +519,12 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -550,7 +541,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -566,15 +557,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -891,21 +890,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -915,352 +914,355 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>104</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3">
-        <f>TestInputData!B4-TestInputData!B5 - TestInputData!B78</f>
+      <c r="B3" s="19">
+        <f>TestInputData!B4-TestInputData!B5 - TestInputData!B77</f>
         <v>999985</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="19"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="18">
         <f>TestInputData!B6</f>
         <v>35000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="18">
+        <f>SUM(TestInputData!B70:B76)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="19">
+        <f>B3-TestInputData!B6-SUM(TestInputData!B70:B76)</f>
+        <v>964915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="20">
+        <f>10*TestInputData!B60</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B6">
-        <f>8*10</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3">
-        <f>B3-TestInputData!B6-TestInputData!B7</f>
-        <v>964905</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="B9" s="20">
         <f>10*TestInputData!B61</f>
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="16">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="20">
         <f>10*TestInputData!B62</f>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="16">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="20">
         <f>10*TestInputData!B63</f>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="16">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="20">
         <f>10*TestInputData!B64</f>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="16">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="20">
         <f>10*TestInputData!B65</f>
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="16">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="20">
         <f>10*TestInputData!B66</f>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="16">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="20">
         <f>10*TestInputData!B67</f>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="16">
-        <f>10*TestInputData!B68</f>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="19">
+        <f>B7-TestInputData!B7</f>
+        <v>959915</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="20">
+        <f>(B7-B17)*TestInputData!B14</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="21">
+        <f>MIN(B17,TestInputData!B20,TestInputData!B22)</f>
+        <v>516500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="21">
+        <f>MIN(B17-B21, TestInputData!B21,TestInputData!B23)</f>
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="B24" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="23">
+        <f>B23*TestInputData!B11</f>
+        <v>19506431.092</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="21">
+        <f>TestInputData!B21-test_modelLogic.py!B23</f>
+        <v>854900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="19">
+        <f>B17-B21-B23</f>
+        <v>348415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="3">
-        <f>B7-TestInputData!B8</f>
-        <v>959905</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="16">
-        <f>(B7-B17)*TestInputData!B15</f>
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="7">
+        <f>B27-(TestInputData!B26/100 *test_modelLogic.py!B3)</f>
+        <v>298415.75</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="11">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="2">
-        <f>MIN(B17,TestInputData!B21,TestInputData!B23)</f>
-        <v>516500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="11">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="2">
-        <f>MIN(B17-B21, TestInputData!B22,TestInputData!B24)</f>
-        <v>95000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="13">
-        <f>B23*TestInputData!B12</f>
-        <v>19506431.092</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="3">
-        <f>B17-B21-B23</f>
-        <v>348405</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="B30" s="14">
+        <f>TestInputData!B27*TestInputData!B28*1000</f>
+        <v>21900500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="7">
-        <f>B26-(TestInputData!B27/100 *test_modelLogic.py!B3)</f>
-        <v>298405.75</v>
-      </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="2">
+        <f>MIN(B29, TestInputData!B34)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="12">
+        <f>B32*TestInputData!B37</f>
+        <v>468093.53240000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="16">
-        <f>TestInputData!B28*TestInputData!B29*1000</f>
-        <v>21900500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="2">
-        <f>MIN(B28, TestInputData!B35)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="14">
-        <f>B31*TestInputData!B38</f>
-        <v>468093.53240000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="2">
-        <f>B5+(B7-B17)+B23+B21+B31+B6</f>
-        <v>652580</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" s="2">
+        <f>B5+(B7-B17)+B23+B21+B32+B6</f>
+        <v>652570</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="15">
-        <f>B34*TestInputData!B16</f>
-        <v>249294165.24617001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="13">
+        <f>B35*TestInputData!B15</f>
+        <v>249290345.11430502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="15">
-        <f>B34*TestInputData!B17</f>
-        <v>189153045.02617002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" s="13">
+        <f>B35*TestInputData!B16</f>
+        <v>189150146.48430502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="17">
-        <f>B34*(TestInputData!B19/100)*TestInputData!B18</f>
-        <v>79756562.338470995</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="B38" s="16">
-        <f>TestInputData!B46*TestInputData!B29*1000</f>
+      <c r="B38" s="15">
+        <f>B35*(TestInputData!B18/100)*TestInputData!B17</f>
+        <v>79755340.165521502</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="14">
+        <f>TestInputData!B45*TestInputData!B28*1000</f>
         <v>175204000</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="13">
+        <f>SUM(B36:B39,B33,B30,B25,B24,B18,B8:B15)</f>
+        <v>735775656.38853157</v>
+      </c>
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>133</v>
-      </c>
-      <c r="B40" s="15">
-        <f>SUM(B35:B38,B32,B29,B25,B24,B18,B8:B15)</f>
-        <v>735783597.23521101</v>
-      </c>
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="5">
-        <f>B28 - B31</f>
-        <v>297405.75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
+      <c r="B43" s="5">
+        <f>B29 - B32</f>
+        <v>297415.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1270,20 +1272,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
@@ -1292,7 +1294,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1324,7 +1326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1333,494 +1335,486 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="B7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>67.76025473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B11" s="10">
-        <v>67.76025473</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>205.33085360000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B12" s="10">
-        <v>205.33085360000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22.927610130000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B13" s="10">
-        <v>22.927610130000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>382.01318650000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B16" s="10">
-        <v>382.01318650000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>289.85418650000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B17" s="10">
-        <v>289.85418650000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244.43458989999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="10">
-        <v>244.43458989999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>88</v>
       </c>
-      <c r="B19">
+      <c r="B18">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3">
+        <v>516500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21">
-        <v>516500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3">
+        <v>949900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3">
+        <v>815000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3">
         <v>95000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23">
-        <v>815000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24">
-        <v>194300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>87602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29">
-        <v>87602</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35">
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>468.09353240000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B38">
-        <v>468.09353240000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>223.87081979999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B39">
-        <v>223.87081979999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>715.70822710000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40">
-        <v>715.70822710000004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>319.9769799</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41">
-        <v>319.9769799</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42">
         <v>1193.9777059999999</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53">
-        <v>-0.12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55">
-        <v>-0.11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56">
-        <v>-0.4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58">
         <v>0.7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>130</v>
-      </c>
-      <c r="B68">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B71">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B72">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B74">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B75">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B76">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B77">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>142</v>
-      </c>
-      <c r="B78">
         <v>10</v>
       </c>
     </row>
@@ -1838,14 +1832,14 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1853,7 +1847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1855,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1877,7 +1871,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1885,7 +1879,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1893,7 +1887,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +1895,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1903,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1917,7 +1911,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1933,7 +1927,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1947,7 +1941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1964,7 +1958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +1971,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1990,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2003,7 +1997,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2016,7 +2010,7 @@
         <v>0.6486508893753401</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2029,7 +2023,7 @@
         <v>0.7026982212493198</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2042,7 +2036,7 @@
         <v>0.80715493680050066</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -2063,7 +2057,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2078,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Updated unit test to accommodate change in long term WMO cost
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repos\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A88EFB-EDD0-4F1C-926D-B742E9593521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814C3A39-7910-4F24-8584-EC67943EC7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,8 +968,8 @@
         <v>113</v>
       </c>
       <c r="B8" s="20">
-        <f>10*TestInputData!B60</f>
-        <v>100</v>
+        <f>10*TestInputData!B60*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -977,8 +977,8 @@
         <v>114</v>
       </c>
       <c r="B9" s="20">
-        <f>10*TestInputData!B61</f>
-        <v>100</v>
+        <f>10*TestInputData!B61*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -986,8 +986,8 @@
         <v>115</v>
       </c>
       <c r="B10" s="20">
-        <f>10*TestInputData!B62</f>
-        <v>100</v>
+        <f>10*TestInputData!B62*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -995,8 +995,8 @@
         <v>116</v>
       </c>
       <c r="B11" s="20">
-        <f>10*TestInputData!B63</f>
-        <v>100</v>
+        <f>10*TestInputData!B63*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1004,8 +1004,8 @@
         <v>117</v>
       </c>
       <c r="B12" s="20">
-        <f>10*TestInputData!B64</f>
-        <v>100</v>
+        <f>10*TestInputData!B64*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1022,8 +1022,8 @@
         <v>119</v>
       </c>
       <c r="B14" s="20">
-        <f>10*TestInputData!B66</f>
-        <v>100</v>
+        <f>10*TestInputData!B66*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1031,8 +1031,8 @@
         <v>120</v>
       </c>
       <c r="B15" s="20">
-        <f>10*TestInputData!B67</f>
-        <v>100</v>
+        <f>10*TestInputData!B67*10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B41" s="13">
         <f>SUM(B36:B39,B33,B30,B25,B24,B18,B8:B15)</f>
-        <v>735775656.38853157</v>
+        <v>735781956.38853157</v>
       </c>
       <c r="C41" s="13"/>
     </row>

</xml_diff>

<commit_message>
Added SWP CVP wheeling costs to water market transfer delivery costs
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repos\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E613E-4AA0-490E-8852-CD1FE5A7BED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA77A1-4364-4E9F-A109-A72363DE00B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
   <sheets>
     <sheet name="test_modelLogic.py" sheetId="2" r:id="rId1"/>
     <sheet name="TestInputData" sheetId="3" r:id="rId2"/>
     <sheet name="test_storageOperations.py" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={71E2AA8F-0F0E-4FF7-9ADE-CEB9B18104B3}</author>
+  </authors>
+  <commentList>
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{71E2AA8F-0F0E-4FF7-9ADE-CEB9B18104B3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Economic loss for this timestep: 373983760.521265</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
   <si>
     <t xml:space="preserve">self.demandsToBeMetByStorage_Contractor </t>
   </si>
@@ -474,6 +492,15 @@
   </si>
   <si>
     <t>Storage Puts Tests</t>
+  </si>
+  <si>
+    <t>totalEconomicLoss_Contractor</t>
+  </si>
+  <si>
+    <t>See "CaUWMET_CPED example for Python test.xslx" for test values</t>
+  </si>
+  <si>
+    <t>totalAnnualCost_Contractor</t>
   </si>
 </sst>
 </file>
@@ -490,7 +517,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +551,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -547,7 +580,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -580,6 +613,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -597,6 +631,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Daly, Kensey" id="{ABA08D6B-941A-49AC-89D5-FF079878CCBC}" userId="S::Kensey.Daly@jacobs.com::2c05a9c7-ae45-4b4b-8861-dac25a878de3" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -894,12 +934,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B46" dT="2023-08-24T15:43:02.96" personId="{ABA08D6B-941A-49AC-89D5-FF079878CCBC}" id="{71E2AA8F-0F0E-4FF7-9ADE-CEB9B18104B3}">
+    <text>Economic loss for this timestep: 373983760.521265</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE31B53E-1762-456C-ABB4-94C4987BBC76}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,6 +955,7 @@
     <col min="1" max="1" width="62.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1184,8 +1233,8 @@
         <v>93</v>
       </c>
       <c r="B33" s="12">
-        <f>B32*TestInputData!B37</f>
-        <v>468093.53240000003</v>
+        <f>B32*(TestInputData!B37 + TestInputData!B14)</f>
+        <v>568093.53239999991</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1249,7 +1298,7 @@
       </c>
       <c r="B41" s="13">
         <f>SUM(B36:B39,B33,B30,B25,B24,B18,B8:B15)</f>
-        <v>735781956.38853157</v>
+        <v>735881956.38853157</v>
       </c>
       <c r="C41" s="13"/>
     </row>
@@ -1267,12 +1316,30 @@
         <v>297415.75</v>
       </c>
     </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="24">
+        <f>B41 + 373983760.521265</f>
+        <v>1109865716.9097965</v>
+      </c>
+    </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1834,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E00A02-92B2-45FA-989E-1582EB4636F5}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated input data and reran model
</commit_message>
<xml_diff>
--- a/CaUWMET/tests/CaUWMET_Tests.xlsx
+++ b/CaUWMET/tests/CaUWMET_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KD012200\GitHub_Repos\California-Urban-Water-Management-Economic-Tool\CaUWMET\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA77A1-4364-4E9F-A109-A72363DE00B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAF6B17-58F5-452C-A069-1913F464167B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C1D8612B-66D0-412C-B825-17E0CA421532}"/>
   </bookViews>
@@ -517,7 +517,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,12 +550,6 @@
       <color rgb="FF6A9955"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -947,7 +941,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,8 +1227,11 @@
         <v>93</v>
       </c>
       <c r="B33" s="12">
-        <f>B32*(TestInputData!B37 + TestInputData!B14)</f>
-        <v>568093.53239999991</v>
+        <f>(B32 * (1+TestInputData!B33/100))*(TestInputData!B37 + TestInputData!B14)</f>
+        <v>670350.36823199992</v>
+      </c>
+      <c r="C33">
+        <v>670350.36823200004</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1298,7 +1295,7 @@
       </c>
       <c r="B41" s="13">
         <f>SUM(B36:B39,B33,B30,B25,B24,B18,B8:B15)</f>
-        <v>735881956.38853157</v>
+        <v>735984213.22436357</v>
       </c>
       <c r="C41" s="13"/>
     </row>
@@ -1330,7 +1327,7 @@
       </c>
       <c r="B46" s="24">
         <f>B41 + 373983760.521265</f>
-        <v>1109865716.9097965</v>
+        <v>1109967973.7456286</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1347,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE42B3F1-5FE2-487D-9208-8AA8C471CD7A}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>